<commit_message>
Leer/Escribir Excel con Apache POI, Matrices de Datos de Prueba
</commit_message>
<xml_diff>
--- a/JavaFramework/src/data/inputData.xlsx
+++ b/JavaFramework/src/data/inputData.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="2985"/>
+    <workbookView windowHeight="2985" windowWidth="14085" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DataTest" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
+    <sheet name="DataTest" r:id="rId1" sheetId="2"/>
+    <sheet name="Hoja2" r:id="rId2" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Componentes</t>
   </si>
@@ -102,12 +102,16 @@
   </si>
   <si>
     <t>lulalipsis258</t>
+  </si>
+  <si>
+    <t>Finalizo OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -196,33 +200,33 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="3" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -239,10 +243,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -400,7 +404,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -409,13 +413,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -425,7 +429,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -434,7 +438,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -443,7 +447,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -453,12 +457,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -489,7 +493,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -508,7 +512,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -520,29 +524,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="29.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="27.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="28.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="20.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="12" max="13" bestFit="true" customWidth="true" style="1" width="29.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="15" max="16384" style="1" width="11.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -567,7 +571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -627,7 +631,10 @@
       </c>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
@@ -672,14 +679,14 @@
       </c>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M6" s="7"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -738,22 +745,22 @@
     <mergeCell ref="B1:M1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="lolipop1216@gmail.com"/>
-    <hyperlink ref="L4" r:id="rId2"/>
+    <hyperlink display="lolipop1216@gmail.com" r:id="rId1" ref="D4"/>
+    <hyperlink r:id="rId2" ref="L4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>